<commit_message>
Changes in location to insert locations inactive because there are funding sources created with some regions already inactive Changes in deliverables:  Creating a field: adopted_licence. Change the null treatment for dissemination channel field. Change the phase name and year option using a new table: bi_phase_by_cubes Changes in funding sources intersect institutions modify `ids_group` from varchar(100) to varchar(200)
</commit_message>
<xml_diff>
--- a/ETLs/config/dim_year.xlsx
+++ b/ETLs/config/dim_year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\MARLO-BI\ETLs\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C567F9-CC0B-448A-8FEC-2898640C516A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562B63FB-90F2-4672-8849-51E6630E5AAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{F6EFAB63-701F-47DD-8F54-FBA5327C12B6}"/>
   </bookViews>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D50BDE6-A6A5-429E-B9AF-AA8A743C11E1}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
         <v>2000</v>
       </c>
       <c r="B2" t="str">
-        <f>TEXT(RIGHT(A2,2),"00")</f>
+        <f t="shared" ref="B2:B17" si="0">TEXT(RIGHT(A2,2),"00")</f>
         <v>00</v>
       </c>
       <c r="C2" s="1">
@@ -436,7 +436,7 @@
         <v>2001</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B41" si="0">TEXT(RIGHT(A3,2),"00")</f>
+        <f t="shared" si="0"/>
         <v>01</v>
       </c>
       <c r="C3" s="1">
@@ -661,7 +661,7 @@
         <v>2016</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B18:B41" si="1">TEXT(RIGHT(A18,2),"00")</f>
         <v>16</v>
       </c>
       <c r="C18" s="1">
@@ -676,7 +676,7 @@
         <v>2017</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C19" s="1">
@@ -691,7 +691,7 @@
         <v>2018</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C20" s="1">
@@ -706,7 +706,7 @@
         <v>2019</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C21" s="1">
@@ -721,7 +721,7 @@
         <v>2020</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="1">
@@ -736,7 +736,7 @@
         <v>2021</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C23" s="1">
@@ -751,7 +751,7 @@
         <v>2022</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C24" s="1">
@@ -766,7 +766,7 @@
         <v>2023</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C25" s="1">
@@ -781,7 +781,7 @@
         <v>2024</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C26" s="1">
@@ -796,7 +796,7 @@
         <v>2025</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C27" s="1">
@@ -811,7 +811,7 @@
         <v>2026</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C28" s="1">
@@ -826,7 +826,7 @@
         <v>2027</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C29" s="1">
@@ -841,7 +841,7 @@
         <v>2028</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" s="1">
@@ -856,7 +856,7 @@
         <v>2029</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C31" s="1">
@@ -871,7 +871,7 @@
         <v>2030</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C32" s="1">
@@ -886,7 +886,7 @@
         <v>2031</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C33" s="1">
@@ -901,7 +901,7 @@
         <v>2032</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C34" s="1">
@@ -916,7 +916,7 @@
         <v>2033</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C35" s="1">
@@ -931,7 +931,7 @@
         <v>2034</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C36" s="1">
@@ -946,7 +946,7 @@
         <v>2035</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" s="1">
@@ -961,7 +961,7 @@
         <v>2036</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" s="1">
@@ -976,7 +976,7 @@
         <v>2037</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C39" s="1">
@@ -991,7 +991,7 @@
         <v>2038</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" s="1">
@@ -1006,7 +1006,7 @@
         <v>2039</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C41" s="1">
@@ -1014,6 +1014,606 @@
       </c>
       <c r="D41" s="1">
         <v>51135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2040</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ref="B42:B81" si="2">TEXT(RIGHT(A42,2),"00")</f>
+        <v>40</v>
+      </c>
+      <c r="C42" s="1">
+        <v>51136</v>
+      </c>
+      <c r="D42" s="1">
+        <v>51501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2041</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="C43" s="1">
+        <v>51502</v>
+      </c>
+      <c r="D43" s="1">
+        <v>51866</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2042</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="C44" s="1">
+        <v>51867</v>
+      </c>
+      <c r="D44" s="1">
+        <v>52231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2043</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="C45" s="1">
+        <v>52232</v>
+      </c>
+      <c r="D45" s="1">
+        <v>52596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2044</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="C46" s="1">
+        <v>52597</v>
+      </c>
+      <c r="D46" s="1">
+        <v>52962</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2045</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="C47" s="1">
+        <v>52963</v>
+      </c>
+      <c r="D47" s="1">
+        <v>53327</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2046</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="C48" s="1">
+        <v>53328</v>
+      </c>
+      <c r="D48" s="1">
+        <v>53692</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2047</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="C49" s="1">
+        <v>53693</v>
+      </c>
+      <c r="D49" s="1">
+        <v>54057</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2048</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="C50" s="1">
+        <v>54058</v>
+      </c>
+      <c r="D50" s="1">
+        <v>54423</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2049</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="C51" s="1">
+        <v>54424</v>
+      </c>
+      <c r="D51" s="1">
+        <v>54788</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2050</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="C52" s="1">
+        <v>54789</v>
+      </c>
+      <c r="D52" s="1">
+        <v>55153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2051</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="C53" s="1">
+        <v>55154</v>
+      </c>
+      <c r="D53" s="1">
+        <v>55518</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2052</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="C54" s="1">
+        <v>55519</v>
+      </c>
+      <c r="D54" s="1">
+        <v>55884</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2053</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="C55" s="1">
+        <v>55885</v>
+      </c>
+      <c r="D55" s="1">
+        <v>56249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2054</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="C56" s="1">
+        <v>56250</v>
+      </c>
+      <c r="D56" s="1">
+        <v>56614</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2055</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="C57" s="1">
+        <v>56615</v>
+      </c>
+      <c r="D57" s="1">
+        <v>56979</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2056</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="C58" s="1">
+        <v>56980</v>
+      </c>
+      <c r="D58" s="1">
+        <v>57345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2057</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="C59" s="1">
+        <v>57346</v>
+      </c>
+      <c r="D59" s="1">
+        <v>57710</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2058</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="C60" s="1">
+        <v>57711</v>
+      </c>
+      <c r="D60" s="1">
+        <v>58075</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2059</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="C61" s="1">
+        <v>58076</v>
+      </c>
+      <c r="D61" s="1">
+        <v>58440</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2060</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="C62" s="1">
+        <v>58441</v>
+      </c>
+      <c r="D62" s="1">
+        <v>58806</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2061</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="C63" s="1">
+        <v>58807</v>
+      </c>
+      <c r="D63" s="1">
+        <v>59171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2062</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="C64" s="1">
+        <v>59172</v>
+      </c>
+      <c r="D64" s="1">
+        <v>59536</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2063</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="C65" s="1">
+        <v>59537</v>
+      </c>
+      <c r="D65" s="1">
+        <v>59901</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2064</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="C66" s="1">
+        <v>59902</v>
+      </c>
+      <c r="D66" s="1">
+        <v>60267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2065</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="C67" s="1">
+        <v>60268</v>
+      </c>
+      <c r="D67" s="1">
+        <v>60632</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2066</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="C68" s="1">
+        <v>60633</v>
+      </c>
+      <c r="D68" s="1">
+        <v>60997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2067</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="C69" s="1">
+        <v>60998</v>
+      </c>
+      <c r="D69" s="1">
+        <v>61362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2068</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="C70" s="1">
+        <v>61363</v>
+      </c>
+      <c r="D70" s="1">
+        <v>61728</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2069</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="C71" s="1">
+        <v>61729</v>
+      </c>
+      <c r="D71" s="1">
+        <v>62093</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2070</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="C72" s="1">
+        <v>62094</v>
+      </c>
+      <c r="D72" s="1">
+        <v>62458</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2071</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="C73" s="1">
+        <v>62459</v>
+      </c>
+      <c r="D73" s="1">
+        <v>62823</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2072</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="C74" s="1">
+        <v>62824</v>
+      </c>
+      <c r="D74" s="1">
+        <v>63189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2073</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="C75" s="1">
+        <v>63190</v>
+      </c>
+      <c r="D75" s="1">
+        <v>63554</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2074</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="C76" s="1">
+        <v>63555</v>
+      </c>
+      <c r="D76" s="1">
+        <v>63919</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2075</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="C77" s="1">
+        <v>63920</v>
+      </c>
+      <c r="D77" s="1">
+        <v>64284</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2076</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="C78" s="1">
+        <v>64285</v>
+      </c>
+      <c r="D78" s="1">
+        <v>64650</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2077</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="C79" s="1">
+        <v>64651</v>
+      </c>
+      <c r="D79" s="1">
+        <v>65015</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2078</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="C80" s="1">
+        <v>65016</v>
+      </c>
+      <c r="D80" s="1">
+        <v>65380</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2079</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="C81" s="1">
+        <v>65381</v>
+      </c>
+      <c r="D81" s="1">
+        <v>65745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>